<commit_message>
Added the new sensitivity ratios calculated from the IEV model spreadsheet modified by exact shifting avoiding double-deployment capex of the 3 technologies (copying and pasting values from [2021:2050] to [2020:2049]). Added lines for comparing the env.py outputs (after reading the new sensitivity ratios) and the extracted reward components from IEV model spreadsheet modified for real world 1-year shifting (copying and pasting values from [2021:2050] to [2020:2049] so that there is double-deployment capex for the 3 technologies).
</commit_message>
<xml_diff>
--- a/environment/sensitivities/IEV - Exact 1-Year Shifting No Double-Deployment - Total Economic Impact.xlsx
+++ b/environment/sensitivities/IEV - Exact 1-Year Shifting No Double-Deployment - Total Economic Impact.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Documents\Work\Research\SAPIENS@SPA-QMUL\TuringProject\RangL-NetZeroTech@MSTeams\General\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BB0AE76-2953-45E2-9B31-CE0E47BD4628}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C38EC330-83FF-4E6B-AE06-0EF2AEB7E15E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34560" windowHeight="15540" xr2:uid="{27067676-B685-42AF-9E82-CB7408D2E7B4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34560" windowHeight="15540" xr2:uid="{BD918F40-6B15-41F2-8534-23101A2115D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -427,16 +427,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD2127F-8B9F-43A3-9598-BEC4044E1136}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8078DBBC-7E35-43CD-ABC1-55844A9486D5}">
   <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="6.88671875" customWidth="1"/>
+    <col min="1" max="1" width="6.77734375" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="6.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -548,97 +548,97 @@
         <v>1</v>
       </c>
       <c r="D2" s="5">
-        <v>39229.256143012761</v>
+        <v>40859.420632815905</v>
       </c>
       <c r="E2" s="5">
-        <v>42217.149901562756</v>
+        <v>44187.036943834777</v>
       </c>
       <c r="F2" s="5">
-        <v>44691.079874149989</v>
+        <v>47817.650747848835</v>
       </c>
       <c r="G2" s="5">
-        <v>48991.181593174217</v>
+        <v>49873.506377285288</v>
       </c>
       <c r="H2" s="5">
-        <v>48617.758165167463</v>
+        <v>51120.813567305828</v>
       </c>
       <c r="I2" s="5">
-        <v>49937.62150251311</v>
+        <v>50096.722198659234</v>
       </c>
       <c r="J2" s="5">
-        <v>48928.377355492441</v>
+        <v>50084.160847639621</v>
       </c>
       <c r="K2" s="5">
-        <v>48734.601315534193</v>
+        <v>50011.964425545011</v>
       </c>
       <c r="L2" s="5">
-        <v>49049.448607077255</v>
+        <v>49234.579054031994</v>
       </c>
       <c r="M2" s="5">
-        <v>48960.316578375699</v>
+        <v>49934.123185134966</v>
       </c>
       <c r="N2" s="5">
-        <v>49771.882927943705</v>
+        <v>49383.486396487031</v>
       </c>
       <c r="O2" s="5">
-        <v>49727.127573881968</v>
+        <v>49416.487444799117</v>
       </c>
       <c r="P2" s="5">
-        <v>48567.124469291724</v>
+        <v>48569.843368840295</v>
       </c>
       <c r="Q2" s="5">
-        <v>49113.582054565166</v>
+        <v>49119.426303352782</v>
       </c>
       <c r="R2" s="5">
-        <v>48378.574580070141</v>
+        <v>48386.631977142213</v>
       </c>
       <c r="S2" s="5">
-        <v>48114.705752009337</v>
+        <v>48122.45031241879</v>
       </c>
       <c r="T2" s="5">
-        <v>48564.594139315494</v>
+        <v>48572.191940919001</v>
       </c>
       <c r="U2" s="5">
-        <v>48895.970456071285</v>
+        <v>48902.63679647744</v>
       </c>
       <c r="V2" s="5">
-        <v>50047.938233566412</v>
+        <v>50056.42591186364</v>
       </c>
       <c r="W2" s="5">
-        <v>51538.075302087695</v>
+        <v>51544.62231777572</v>
       </c>
       <c r="X2" s="5">
-        <v>53287.091045068941</v>
+        <v>53295.086497048775</v>
       </c>
       <c r="Y2" s="5">
-        <v>55099.405484199451</v>
+        <v>55106.412265273699</v>
       </c>
       <c r="Z2" s="5">
-        <v>57027.875245340168</v>
+        <v>57035.834493365299</v>
       </c>
       <c r="AA2" s="5">
-        <v>59188.230752505275</v>
+        <v>59195.569177382757</v>
       </c>
       <c r="AB2" s="5">
-        <v>61595.951871905228</v>
+        <v>61603.457081555141</v>
       </c>
       <c r="AC2" s="5">
-        <v>64269.511376371069</v>
+        <v>64278.985233287152</v>
       </c>
       <c r="AD2" s="5">
-        <v>67236.758158228258</v>
+        <v>67243.385076759383</v>
       </c>
       <c r="AE2" s="5">
-        <v>70512.10910527948</v>
+        <v>70519.710151723702</v>
       </c>
       <c r="AF2" s="5">
-        <v>73792.205965306697</v>
+        <v>73793.579028871856</v>
       </c>
       <c r="AG2" s="5">
-        <v>77508.436869221478</v>
+        <v>77510.96537933698</v>
       </c>
       <c r="AH2" s="5">
-        <v>78517.412529127469</v>
+        <v>78516.39435377231</v>
       </c>
     </row>
     <row r="3" spans="1:34" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -652,97 +652,97 @@
         <v>1</v>
       </c>
       <c r="D3" s="5">
-        <v>39228.934745875093</v>
+        <v>40862.01489470368</v>
       </c>
       <c r="E3" s="5">
-        <v>42248.343250141617</v>
+        <v>44201.626775360979</v>
       </c>
       <c r="F3" s="5">
-        <v>44718.324725359023</v>
+        <v>47843.88446701513</v>
       </c>
       <c r="G3" s="5">
-        <v>49032.661818897206</v>
+        <v>49914.041849709523</v>
       </c>
       <c r="H3" s="5">
-        <v>48676.793528284477</v>
+        <v>51179.050835423972</v>
       </c>
       <c r="I3" s="5">
-        <v>49987.255454617472</v>
+        <v>50145.970265619981</v>
       </c>
       <c r="J3" s="5">
-        <v>48991.34273215205</v>
+        <v>50146.052203292857</v>
       </c>
       <c r="K3" s="5">
-        <v>48813.928511235827</v>
+        <v>50090.447243408475</v>
       </c>
       <c r="L3" s="5">
-        <v>49148.926718305214</v>
+        <v>49528.471662976452</v>
       </c>
       <c r="M3" s="5">
-        <v>49491.322633903488</v>
+        <v>50544.039016916133</v>
       </c>
       <c r="N3" s="5">
-        <v>50701.236879347634</v>
+        <v>50801.781098555133</v>
       </c>
       <c r="O3" s="5">
-        <v>52034.061450446337</v>
+        <v>51400.160720835585</v>
       </c>
       <c r="P3" s="5">
-        <v>51078.232755132165</v>
+        <v>51082.369616023869</v>
       </c>
       <c r="Q3" s="5">
-        <v>52285.241009484569</v>
+        <v>52288.820890633375</v>
       </c>
       <c r="R3" s="5">
-        <v>52077.752389089554</v>
+        <v>52085.823076441608</v>
       </c>
       <c r="S3" s="5">
-        <v>52385.353695350357</v>
+        <v>52390.864019469431</v>
       </c>
       <c r="T3" s="5">
-        <v>53516.156896280052</v>
+        <v>53524.151723899937</v>
       </c>
       <c r="U3" s="5">
-        <v>54511.823825152576</v>
+        <v>54516.484372305131</v>
       </c>
       <c r="V3" s="5">
-        <v>56493.39213352534</v>
+        <v>56499.742904772596</v>
       </c>
       <c r="W3" s="5">
-        <v>58901.787126466843</v>
+        <v>58907.114994096628</v>
       </c>
       <c r="X3" s="5">
-        <v>61646.88043205491</v>
+        <v>61654.775857585031</v>
       </c>
       <c r="Y3" s="5">
-        <v>64530.732333633685</v>
+        <v>64536.664484045694</v>
       </c>
       <c r="Z3" s="5">
-        <v>67564.259052098656</v>
+        <v>67573.856683828824</v>
       </c>
       <c r="AA3" s="5">
-        <v>70903.480431550619</v>
+        <v>70910.046134453631</v>
       </c>
       <c r="AB3" s="5">
-        <v>74555.903899424127</v>
+        <v>74562.07264932667</v>
       </c>
       <c r="AC3" s="5">
-        <v>78541.300810084664</v>
+        <v>78547.046915107465</v>
       </c>
       <c r="AD3" s="5">
-        <v>82874.188774801485</v>
+        <v>82881.682724827755</v>
       </c>
       <c r="AE3" s="5">
-        <v>87577.432861993671</v>
+        <v>87581.968508913822</v>
       </c>
       <c r="AF3" s="5">
-        <v>91515.50538895691</v>
+        <v>91517.894866016242</v>
       </c>
       <c r="AG3" s="5">
-        <v>96153.610900334941</v>
+        <v>96155.712867188748</v>
       </c>
       <c r="AH3" s="5">
-        <v>94940.951139353623</v>
+        <v>94937.812154554253</v>
       </c>
     </row>
     <row r="4" spans="1:34" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -756,97 +756,97 @@
         <v>1</v>
       </c>
       <c r="D4" s="5">
-        <v>39228.934745875093</v>
+        <v>40866.316920224788</v>
       </c>
       <c r="E4" s="5">
-        <v>42326.799183198549</v>
+        <v>44236.36014906122</v>
       </c>
       <c r="F4" s="5">
-        <v>44783.283683038258</v>
+        <v>47906.287099993322</v>
       </c>
       <c r="G4" s="5">
-        <v>49131.483651738978</v>
+        <v>50010.773619032028</v>
       </c>
       <c r="H4" s="5">
-        <v>48816.334166565357</v>
+        <v>51317.74751145659</v>
       </c>
       <c r="I4" s="5">
-        <v>50106.664733891048</v>
+        <v>50263.285464175278</v>
       </c>
       <c r="J4" s="5">
-        <v>49139.271694824201</v>
+        <v>50293.446915616048</v>
       </c>
       <c r="K4" s="5">
-        <v>49002.774976661196</v>
+        <v>50277.471133678104</v>
       </c>
       <c r="L4" s="5">
-        <v>49381.273584582625</v>
+        <v>49919.32687037759</v>
       </c>
       <c r="M4" s="5">
-        <v>50113.225818106475</v>
+        <v>51229.6988342185</v>
       </c>
       <c r="N4" s="5">
-        <v>51653.257236345889</v>
+        <v>52148.417755495495</v>
       </c>
       <c r="O4" s="5">
-        <v>54176.262273785731</v>
+        <v>53279.13168361954</v>
       </c>
       <c r="P4" s="5">
-        <v>53481.141264764789</v>
+        <v>53484.277576406559</v>
       </c>
       <c r="Q4" s="5">
-        <v>55339.334144850145</v>
+        <v>55344.948066308381</v>
       </c>
       <c r="R4" s="5">
-        <v>55702.710845483118</v>
+        <v>55708.095418743149</v>
       </c>
       <c r="S4" s="5">
-        <v>56625.979798425673</v>
+        <v>56632.911874979945</v>
       </c>
       <c r="T4" s="5">
-        <v>58507.548042350711</v>
+        <v>58513.090819570898</v>
       </c>
       <c r="U4" s="5">
-        <v>60253.821597402493</v>
+        <v>60257.555659773076</v>
       </c>
       <c r="V4" s="5">
-        <v>63174.09722372063</v>
+        <v>63181.743818835806</v>
       </c>
       <c r="W4" s="5">
-        <v>66645.661511570695</v>
+        <v>66652.923661231558</v>
       </c>
       <c r="X4" s="5">
-        <v>70574.553758756403</v>
+        <v>70583.141297985392</v>
       </c>
       <c r="Y4" s="5">
-        <v>74762.417190649838</v>
+        <v>74768.218495457375</v>
       </c>
       <c r="Z4" s="5">
-        <v>79190.717843921011</v>
+        <v>79198.225511313984</v>
       </c>
       <c r="AA4" s="5">
-        <v>84051.32789393836</v>
+        <v>84056.189404497884</v>
       </c>
       <c r="AB4" s="5">
-        <v>89360.730929573867</v>
+        <v>89366.054495107528</v>
       </c>
       <c r="AC4" s="5">
-        <v>95143.614741422862</v>
+        <v>95150.494274590921</v>
       </c>
       <c r="AD4" s="5">
-        <v>101424.84875701205</v>
+        <v>101429.7771915824</v>
       </c>
       <c r="AE4" s="5">
-        <v>108218.13393042824</v>
+        <v>108220.2728036975</v>
       </c>
       <c r="AF4" s="5">
-        <v>113109.55842538064</v>
+        <v>113110.91633989454</v>
       </c>
       <c r="AG4" s="5">
-        <v>119135.73261199678</v>
+        <v>119135.88353016907</v>
       </c>
       <c r="AH4" s="5">
-        <v>114306.82177483599</v>
+        <v>114304.84327530439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>